<commit_message>
Versão 3.4 gráficos de casos por região salvando jpeg
</commit_message>
<xml_diff>
--- a/criterios_por_tipo.xlsx
+++ b/criterios_por_tipo.xlsx
@@ -672,21 +672,51 @@
           <t>Não se aplica</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
-      <c r="P5" t="inlineStr"/>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>